<commit_message>
Added tabs to the dashboard and updated rubrix/README
</commit_message>
<xml_diff>
--- a/ProjectRubric.xlsx
+++ b/ProjectRubric.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukemcconnell/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukemcconnell/Desktop/UT Semester 10/544 - Decision Support Systems/Python/Dash_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC125FC-06A1-2E40-8087-B2C432FFF519}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6118BF-6FB8-6E46-843B-C0A998DA6F23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="480" windowWidth="25320" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,19 +160,6 @@
   </si>
   <si>
     <r>
-      <t>5+ distinct</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve"> (dcc.Dropdown, dcc.RangeSlider, dcc.RadioItems, dcc.Graph) - NEEED 1 MORE?</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">3+ </t>
     </r>
     <r>
@@ -182,19 +169,6 @@
         <rFont val="Calibri (Body)"/>
       </rPr>
       <t>(graph 1, graph 2, logos/links)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Appropriate organization of code.  Appropriate comments. If I am looking for code, is it where it should be?  Can I read all of the code? If not, are there at least appropriate comments? </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>(make sure call backs have comments)</t>
     </r>
   </si>
   <si>
@@ -229,6 +203,22 @@
         <rFont val="Calibri (Body)"/>
       </rPr>
       <t>(Do logos/links count as a graphic, or do we need to add another?)</t>
+    </r>
+  </si>
+  <si>
+    <t>Appropriate organization of code.  Appropriate comments. If I am looking for code, is it where it should be?  Can I read all of the code? If not, are there at least appropriate comments?</t>
+  </si>
+  <si>
+    <r>
+      <t>5+ distinct</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> (dcc.Dropdown, dcc.RangeSlider, dcc.RadioItems, dcc.Graph, dcc.Tab)</t>
     </r>
   </si>
 </sst>
@@ -513,7 +503,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -581,6 +571,39 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -608,41 +631,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -926,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -938,16 +931,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="38"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="30"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="39"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="41"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="33"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="12"/>
@@ -963,12 +956,12 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="45"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="37"/>
       <c r="E4" s="11"/>
     </row>
     <row r="5" spans="1:10" ht="30" customHeight="1">
@@ -1006,14 +999,14 @@
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="46">
-        <v>8</v>
+      <c r="C7" s="48">
+        <v>10</v>
       </c>
       <c r="D7" s="19">
         <v>10</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1028,7 +1021,7 @@
         <v>10</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1043,7 +1036,7 @@
         <v>5</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1">
@@ -1051,7 +1044,9 @@
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="47"/>
+      <c r="C10" s="47">
+        <v>4</v>
+      </c>
       <c r="D10" s="18">
         <v>4</v>
       </c>
@@ -1098,8 +1093,8 @@
       <c r="D13" s="19">
         <v>5</v>
       </c>
-      <c r="E13" s="42" t="s">
-        <v>41</v>
+      <c r="E13" s="34" t="s">
+        <v>39</v>
       </c>
       <c r="J13" s="15"/>
     </row>
@@ -1114,18 +1109,18 @@
       <c r="D14" s="19">
         <v>5</v>
       </c>
-      <c r="E14" s="42"/>
+      <c r="E14" s="34"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="5"/>
       <c r="B15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="46"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="19">
         <v>5</v>
       </c>
-      <c r="E15" s="42"/>
+      <c r="E15" s="34"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="5"/>
@@ -1141,13 +1136,13 @@
       <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="28"/>
+      <c r="B17" s="39"/>
       <c r="C17" s="24">
         <f>C5*SUM(C6:C16)</f>
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D17" s="20">
         <f>D5*SUM(D6:D16)</f>
@@ -1157,12 +1152,12 @@
     </row>
     <row r="18" spans="1:5" ht="3" customHeight="1"/>
     <row r="19" spans="1:5">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="35"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="46"/>
       <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5">
@@ -1240,10 +1235,10 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="28"/>
+      <c r="B26" s="39"/>
       <c r="C26" s="24">
         <f>SUM(C20:C25)</f>
         <v>0</v>
@@ -1256,10 +1251,10 @@
     </row>
     <row r="27" spans="1:5" ht="3.75" customHeight="1"/>
     <row r="28" spans="1:5" ht="30" customHeight="1">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="30"/>
+      <c r="B28" s="41"/>
       <c r="C28" s="25"/>
       <c r="D28" s="10">
         <v>12</v>
@@ -1267,10 +1262,10 @@
     </row>
     <row r="29" spans="1:5" ht="3" customHeight="1"/>
     <row r="30" spans="1:5" ht="45.75" customHeight="1">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="32"/>
+      <c r="B30" s="43"/>
       <c r="C30" s="25"/>
       <c r="D30" s="10">
         <v>8</v>
@@ -1287,13 +1282,13 @@
       <c r="E31" s="17"/>
     </row>
     <row r="32" spans="1:5" ht="30" customHeight="1" thickBot="1">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="34"/>
+      <c r="B32" s="45"/>
       <c r="C32" s="26">
         <f>C17 + C26 +C28+C30</f>
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D32" s="21">
         <f>D17 + D26 +D28+D30</f>
@@ -1302,15 +1297,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A19:D19"/>
     <mergeCell ref="A1:C2"/>
     <mergeCell ref="E13:E15"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A19:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added new graph and updated rubric
</commit_message>
<xml_diff>
--- a/ProjectRubric.xlsx
+++ b/ProjectRubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukemcconnell/Desktop/UT Semester 10/544 - Decision Support Systems/Python/Dash_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6118BF-6FB8-6E46-843B-C0A998DA6F23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E63674-CB40-774A-898B-4E347ED12517}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="480" windowWidth="25320" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,6 +169,22 @@
         <rFont val="Calibri (Body)"/>
       </rPr>
       <t>(graph 1, graph 2, logos/links)</t>
+    </r>
+  </si>
+  <si>
+    <t>Appropriate organization of code.  Appropriate comments. If I am looking for code, is it where it should be?  Can I read all of the code? If not, are there at least appropriate comments?</t>
+  </si>
+  <si>
+    <r>
+      <t>5+ distinct</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> (dcc.Dropdown, dcc.RangeSlider, dcc.RadioItems, dcc.Graph, dcc.Tab)</t>
     </r>
   </si>
   <si>
@@ -202,23 +218,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>(Do logos/links count as a graphic, or do we need to add another?)</t>
-    </r>
-  </si>
-  <si>
-    <t>Appropriate organization of code.  Appropriate comments. If I am looking for code, is it where it should be?  Can I read all of the code? If not, are there at least appropriate comments?</t>
-  </si>
-  <si>
-    <r>
-      <t>5+ distinct</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve"> (dcc.Dropdown, dcc.RangeSlider, dcc.RadioItems, dcc.Graph, dcc.Tab)</t>
+      <t>(4 graphs, logos with links as well)</t>
     </r>
   </si>
 </sst>
@@ -256,19 +256,13 @@
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -503,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -571,8 +565,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -608,33 +626,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -919,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:E15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -931,16 +922,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="30"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="38"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="31"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="41"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="12"/>
@@ -956,12 +947,12 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="37"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="45"/>
       <c r="E4" s="11"/>
     </row>
     <row r="5" spans="1:10" ht="30" customHeight="1">
@@ -999,14 +990,14 @@
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="48">
+      <c r="C7" s="28">
         <v>10</v>
       </c>
       <c r="D7" s="19">
         <v>10</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1044,14 +1035,14 @@
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="47">
+      <c r="C10" s="27">
         <v>4</v>
       </c>
       <c r="D10" s="18">
         <v>4</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1093,8 +1084,8 @@
       <c r="D13" s="19">
         <v>5</v>
       </c>
-      <c r="E13" s="34" t="s">
-        <v>39</v>
+      <c r="E13" s="42" t="s">
+        <v>41</v>
       </c>
       <c r="J13" s="15"/>
     </row>
@@ -1109,18 +1100,20 @@
       <c r="D14" s="19">
         <v>5</v>
       </c>
-      <c r="E14" s="34"/>
+      <c r="E14" s="42"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="5"/>
       <c r="B15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="27"/>
+      <c r="C15" s="28">
+        <v>5</v>
+      </c>
       <c r="D15" s="19">
         <v>5</v>
       </c>
-      <c r="E15" s="34"/>
+      <c r="E15" s="42"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="5"/>
@@ -1136,13 +1129,13 @@
       <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="39"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="24">
         <f>C5*SUM(C6:C16)</f>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D17" s="20">
         <f>D5*SUM(D6:D16)</f>
@@ -1152,12 +1145,12 @@
     </row>
     <row r="18" spans="1:5" ht="3" customHeight="1"/>
     <row r="19" spans="1:5">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="46"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="35"/>
       <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5">
@@ -1235,10 +1228,10 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="39"/>
+      <c r="B26" s="47"/>
       <c r="C26" s="24">
         <f>SUM(C20:C25)</f>
         <v>0</v>
@@ -1251,10 +1244,10 @@
     </row>
     <row r="27" spans="1:5" ht="3.75" customHeight="1"/>
     <row r="28" spans="1:5" ht="30" customHeight="1">
-      <c r="A28" s="40" t="s">
+      <c r="A28" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="41"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="25"/>
       <c r="D28" s="10">
         <v>12</v>
@@ -1262,10 +1255,10 @@
     </row>
     <row r="29" spans="1:5" ht="3" customHeight="1"/>
     <row r="30" spans="1:5" ht="45.75" customHeight="1">
-      <c r="A30" s="42" t="s">
+      <c r="A30" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="43"/>
+      <c r="B30" s="32"/>
       <c r="C30" s="25"/>
       <c r="D30" s="10">
         <v>8</v>
@@ -1282,13 +1275,13 @@
       <c r="E31" s="17"/>
     </row>
     <row r="32" spans="1:5" ht="30" customHeight="1" thickBot="1">
-      <c r="A32" s="44" t="s">
+      <c r="A32" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="45"/>
+      <c r="B32" s="34"/>
       <c r="C32" s="26">
         <f>C17 + C26 +C28+C30</f>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D32" s="21">
         <f>D17 + D26 +D28+D30</f>
@@ -1297,15 +1290,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A26:B26"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A1:C2"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A26:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added diagram to technical summary
</commit_message>
<xml_diff>
--- a/ProjectRubric.xlsx
+++ b/ProjectRubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukemcconnell/Desktop/UT Semester 10/544 - Decision Support Systems/Python/Dash_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E63674-CB40-774A-898B-4E347ED12517}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A4EEDB-F1AE-8743-A3FC-6A50621491B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="480" windowWidth="25320" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -571,6 +571,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -609,24 +627,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -911,7 +911,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -922,16 +922,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="38"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="44"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="39"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="41"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="47"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="12"/>
@@ -947,12 +947,12 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="45"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="32"/>
       <c r="E4" s="11"/>
     </row>
     <row r="5" spans="1:10" ht="30" customHeight="1">
@@ -1084,7 +1084,7 @@
       <c r="D13" s="19">
         <v>5</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="29" t="s">
         <v>41</v>
       </c>
       <c r="J13" s="15"/>
@@ -1100,7 +1100,7 @@
       <c r="D14" s="19">
         <v>5</v>
       </c>
-      <c r="E14" s="42"/>
+      <c r="E14" s="29"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="5"/>
@@ -1113,7 +1113,7 @@
       <c r="D15" s="19">
         <v>5</v>
       </c>
-      <c r="E15" s="42"/>
+      <c r="E15" s="29"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="5"/>
@@ -1129,10 +1129,10 @@
       <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="47"/>
+      <c r="B17" s="34"/>
       <c r="C17" s="24">
         <f>C5*SUM(C6:C16)</f>
         <v>60</v>
@@ -1145,12 +1145,12 @@
     </row>
     <row r="18" spans="1:5" ht="3" customHeight="1"/>
     <row r="19" spans="1:5">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="35"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="41"/>
       <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5">
@@ -1228,10 +1228,10 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="46" t="s">
+      <c r="A26" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="47"/>
+      <c r="B26" s="34"/>
       <c r="C26" s="24">
         <f>SUM(C20:C25)</f>
         <v>0</v>
@@ -1244,21 +1244,23 @@
     </row>
     <row r="27" spans="1:5" ht="3.75" customHeight="1"/>
     <row r="28" spans="1:5" ht="30" customHeight="1">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="25"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="25">
+        <v>12</v>
+      </c>
       <c r="D28" s="10">
         <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="3" customHeight="1"/>
     <row r="30" spans="1:5" ht="45.75" customHeight="1">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="32"/>
+      <c r="B30" s="38"/>
       <c r="C30" s="25"/>
       <c r="D30" s="10">
         <v>8</v>
@@ -1275,13 +1277,13 @@
       <c r="E31" s="17"/>
     </row>
     <row r="32" spans="1:5" ht="30" customHeight="1" thickBot="1">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="34"/>
+      <c r="B32" s="40"/>
       <c r="C32" s="26">
         <f>C17 + C26 +C28+C30</f>
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="D32" s="21">
         <f>D17 + D26 +D28+D30</f>
@@ -1290,15 +1292,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A1:C2"/>
     <mergeCell ref="E13:E15"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A1:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>